<commit_message>
quick update for making tags
</commit_message>
<xml_diff>
--- a/planting/freezing_planting.xlsx
+++ b/planting/freezing_planting.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28460" yWindow="1940" windowWidth="24960" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="18600" yWindow="2500" windowWidth="24960" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -403,16 +403,13 @@
   </si>
   <si>
     <t>yellow</t>
-  </si>
-  <si>
-    <t>raised beds?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -439,6 +436,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -748,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53:I99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2007,7 +2010,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -2110,11 +2113,8 @@
       <c r="H52" t="s">
         <v>122</v>
       </c>
-      <c r="I52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -2139,11 +2139,8 @@
       <c r="H53" t="s">
         <v>122</v>
       </c>
-      <c r="I53" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
@@ -2168,11 +2165,8 @@
       <c r="H54" t="s">
         <v>122</v>
       </c>
-      <c r="I54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
@@ -2197,11 +2191,8 @@
       <c r="H55" t="s">
         <v>123</v>
       </c>
-      <c r="I55" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -2226,11 +2217,8 @@
       <c r="H56" t="s">
         <v>122</v>
       </c>
-      <c r="I56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>72</v>
       </c>
@@ -2255,11 +2243,8 @@
       <c r="H57" t="s">
         <v>122</v>
       </c>
-      <c r="I57" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>73</v>
       </c>
@@ -2284,11 +2269,8 @@
       <c r="H58" t="s">
         <v>122</v>
       </c>
-      <c r="I58" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>74</v>
       </c>
@@ -2313,11 +2295,8 @@
       <c r="H59" t="s">
         <v>123</v>
       </c>
-      <c r="I59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>75</v>
       </c>
@@ -2342,11 +2321,8 @@
       <c r="H60" t="s">
         <v>123</v>
       </c>
-      <c r="I60" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -2371,11 +2347,8 @@
       <c r="H61" t="s">
         <v>122</v>
       </c>
-      <c r="I61" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>77</v>
       </c>
@@ -2400,11 +2373,8 @@
       <c r="H62" t="s">
         <v>122</v>
       </c>
-      <c r="I62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
@@ -2429,11 +2399,8 @@
       <c r="H63" t="s">
         <v>122</v>
       </c>
-      <c r="I63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>79</v>
       </c>
@@ -2458,11 +2425,8 @@
       <c r="H64" t="s">
         <v>122</v>
       </c>
-      <c r="I64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>80</v>
       </c>
@@ -2487,11 +2451,8 @@
       <c r="H65" t="s">
         <v>122</v>
       </c>
-      <c r="I65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>81</v>
       </c>
@@ -2516,11 +2477,8 @@
       <c r="H66" t="s">
         <v>123</v>
       </c>
-      <c r="I66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>82</v>
       </c>
@@ -2545,11 +2503,8 @@
       <c r="H67" t="s">
         <v>123</v>
       </c>
-      <c r="I67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>83</v>
       </c>
@@ -2574,11 +2529,8 @@
       <c r="H68" t="s">
         <v>122</v>
       </c>
-      <c r="I68" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>84</v>
       </c>
@@ -2603,11 +2555,8 @@
       <c r="H69" t="s">
         <v>123</v>
       </c>
-      <c r="I69" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>85</v>
       </c>
@@ -2632,11 +2581,8 @@
       <c r="H70" t="s">
         <v>123</v>
       </c>
-      <c r="I70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>86</v>
       </c>
@@ -2661,11 +2607,8 @@
       <c r="H71" t="s">
         <v>123</v>
       </c>
-      <c r="I71" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>87</v>
       </c>
@@ -2690,11 +2633,8 @@
       <c r="H72" t="s">
         <v>123</v>
       </c>
-      <c r="I72" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>88</v>
       </c>
@@ -2719,11 +2659,8 @@
       <c r="H73" t="s">
         <v>122</v>
       </c>
-      <c r="I73" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>89</v>
       </c>
@@ -2748,11 +2685,8 @@
       <c r="H74" t="s">
         <v>122</v>
       </c>
-      <c r="I74" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>90</v>
       </c>
@@ -2777,11 +2711,8 @@
       <c r="H75" t="s">
         <v>122</v>
       </c>
-      <c r="I75" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>91</v>
       </c>
@@ -2806,11 +2737,8 @@
       <c r="H76" t="s">
         <v>123</v>
       </c>
-      <c r="I76" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>92</v>
       </c>
@@ -2835,11 +2763,8 @@
       <c r="H77" t="s">
         <v>123</v>
       </c>
-      <c r="I77" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>93</v>
       </c>
@@ -2864,11 +2789,8 @@
       <c r="H78" t="s">
         <v>122</v>
       </c>
-      <c r="I78" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>94</v>
       </c>
@@ -2893,11 +2815,8 @@
       <c r="H79" t="s">
         <v>122</v>
       </c>
-      <c r="I79" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>95</v>
       </c>
@@ -2922,11 +2841,8 @@
       <c r="H80" t="s">
         <v>123</v>
       </c>
-      <c r="I80" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>96</v>
       </c>
@@ -2951,11 +2867,8 @@
       <c r="H81" t="s">
         <v>122</v>
       </c>
-      <c r="I81" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>97</v>
       </c>
@@ -2980,11 +2893,8 @@
       <c r="H82" t="s">
         <v>122</v>
       </c>
-      <c r="I82" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>98</v>
       </c>
@@ -3009,11 +2919,8 @@
       <c r="H83" t="s">
         <v>122</v>
       </c>
-      <c r="I83" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>99</v>
       </c>
@@ -3038,11 +2945,8 @@
       <c r="H84" t="s">
         <v>123</v>
       </c>
-      <c r="I84" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>100</v>
       </c>
@@ -3067,11 +2971,8 @@
       <c r="H85" t="s">
         <v>122</v>
       </c>
-      <c r="I85" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>101</v>
       </c>
@@ -3096,11 +2997,8 @@
       <c r="H86" t="s">
         <v>122</v>
       </c>
-      <c r="I86" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>102</v>
       </c>
@@ -3125,11 +3023,8 @@
       <c r="H87" t="s">
         <v>122</v>
       </c>
-      <c r="I87" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>103</v>
       </c>
@@ -3154,11 +3049,8 @@
       <c r="H88" t="s">
         <v>122</v>
       </c>
-      <c r="I88" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>104</v>
       </c>
@@ -3183,11 +3075,8 @@
       <c r="H89" t="s">
         <v>123</v>
       </c>
-      <c r="I89" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>105</v>
       </c>
@@ -3212,11 +3101,8 @@
       <c r="H90" t="s">
         <v>123</v>
       </c>
-      <c r="I90" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>106</v>
       </c>
@@ -3241,11 +3127,8 @@
       <c r="H91" t="s">
         <v>123</v>
       </c>
-      <c r="I91" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>107</v>
       </c>
@@ -3270,11 +3153,8 @@
       <c r="H92" t="s">
         <v>123</v>
       </c>
-      <c r="I92" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>108</v>
       </c>
@@ -3299,11 +3179,8 @@
       <c r="H93" t="s">
         <v>122</v>
       </c>
-      <c r="I93" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>109</v>
       </c>
@@ -3328,11 +3205,8 @@
       <c r="H94" t="s">
         <v>123</v>
       </c>
-      <c r="I94" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>110</v>
       </c>
@@ -3357,11 +3231,8 @@
       <c r="H95" t="s">
         <v>123</v>
       </c>
-      <c r="I95" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>111</v>
       </c>
@@ -3386,11 +3257,8 @@
       <c r="H96" t="s">
         <v>123</v>
       </c>
-      <c r="I96" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>112</v>
       </c>
@@ -3415,11 +3283,8 @@
       <c r="H97" t="s">
         <v>122</v>
       </c>
-      <c r="I97" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>113</v>
       </c>
@@ -3444,11 +3309,8 @@
       <c r="H98" t="s">
         <v>123</v>
       </c>
-      <c r="I98" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>114</v>
       </c>
@@ -3473,13 +3335,13 @@
       <c r="H99" t="s">
         <v>123</v>
       </c>
-      <c r="I99" t="s">
-        <v>124</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>